<commit_message>
feat: implement file upload&download
</commit_message>
<xml_diff>
--- a/backend/data/test.xlsx
+++ b/backend/data/test.xlsx
@@ -86,61 +86,61 @@
     <t>전문가가 설계한 느낌</t>
   </si>
   <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러움\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; &lt;이용,  좋다&gt;&lt;/s&gt;&lt;/s&gt; &lt;향, 좋다&gt;&lt;/s&gt;禮)&lt;/s&gt; 한다&gt;&lt;/s&gt; 한다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; Insode&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n디자인\n\n### Response(응답):&lt;디자인, 좋다&gt;&lt;/s&gt; 한다&gt;&lt;/s&gt; 한다&gt;&lt;/s&gt;丸,&lt;/s&gt; 한다&gt;&lt;/s&gt; 한다&gt;&lt;/s&gt;&lt;/s&gt;泥田&gt;&lt;/s&gt;&lt;/s&gt; 한다&gt;&lt;/s&gt;utylutose&gt;&lt;/s&gt;敾泥泥窟, 선호 있다고&gt;&lt;/s&gt;&lt;/s&gt;ut']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; 시주잔여 시주잔여 주기, 좋다&gt;&lt;/s&gt; 시주잔여 주기, 좋다&gt;&lt;/s&gt;&lt;/s&gt; &lt;靑磁&lt;/s&gt;oria&lt;/s&gt;ental&gt;&lt;/s&gt; 참&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; Ins']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n삼성이라는 브랜드\n\n### Response(응답):&lt;브랜드, 좋다&gt;&lt;/s&gt;臺 &lt;신발, 좋다&gt;&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺拓臺&lt;/s&gt;臺)&lt;/s&gt;臺&lt;/s&gt;臺)&lt;/s&gt;臺 &lt;선 신발, 인상']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n전문건설업체시공\n\n### Response(응답):&lt;업체, 전문적이다&gt;&lt;/s&gt; &lt;이용, 편하다&gt;&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏炭梨&lt;/s&gt;裏辰出, 예쁘게 된다&gt;&lt;/s&gt;裏辰&lt;/s&gt; 결정되었다.\n&lt;/s&gt;裏振&lt;/s&gt; 결정되었다.\n&lt;/s&gt; 결정되었다.\n&lt;/s&gt;']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n가장 유명한 브랜드라서\n\n### Response(응답):&lt;브랜드, 유명하다&gt;&lt;/s&gt;籤, 잘된다&gt;&lt;/s&gt;粒, 잘된다&gt;&lt;/s&gt; 잘 깬다&gt;&lt;/s&gt; 잘 깬다&gt;&lt;/s&gt; 잘 깬다&gt;&lt;/s&gt; 잘 깬다&gt;&lt;/s&gt; 잘 깬다&gt;&lt;/s&gt; 잘']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n튼튼하교 깨끗\n\n### Response(응답):&lt;NULL, 튼튼하다&gt; &lt;NULL, 깨끗하다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;oria&lt;/s&gt;oria tuntelber)이라고도 할 참조).\n&lt;/s&gt;oria tylove &lt;설 &lt;신발, 참신하다&gt;&lt;/s&gt;oria']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n현대라는 회사가 믿을수 있어서\n\n### Response(응답):&lt;회사, 믿음이 간다&gt;&lt;/s&gt;臺 &lt;신발, 좋다&gt;&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;台&lt;/s&gt;臺 &lt;&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺)&lt;/s&gt; 참 인상적이지 않']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; 시주한다&gt;&lt;/s&gt;丸, 대주로 사용한다&gt;&lt;/s&gt;珠&lt;/s&gt;主)&lt;/s&gt;&lt;/s&gt;珠&lt;/s&gt;柱)&lt;/s&gt;珠&lt;/s&gt;晋&lt;/s&gt;珠&lt;/s&gt;鎭)&lt;/s&gt;珠&lt;/s&gt;柱)&lt;/s&gt;珠&lt;/s&gt;&lt;/s&gt; 주 의뢰']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스럽다\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; &lt;이용,  용이하다&gt;&lt;/s&gt; 비판하였다.\n한다&gt;&lt;/s&gt; 비판하였다.\n&lt;/s&gt; 비판하였다.\n한다&gt;&lt;/s&gt; 비판하였다.\n &lt;향, 비판하였다.\n한다&gt;&lt;/s&gt; 요구하였다.\n한다&gt;&lt;/s&gt; 당하였다.\n&gt;&lt;/s&gt; 변경하여 주장하였다.\n&lt;/s&gt;&lt;/s&gt; 체결하였다.\n']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 이미지\n\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;梨, 예쁘다&gt;&lt;/s&gt;尤&lt;/s&gt;ric, 예쁘다&gt;&lt;/s&gt;orea&gt;&lt;/s&gt;ite&lt;/s&gt;entality &lt;선, 예쁘다&gt;&lt;/s&gt;&lt;/s&gt;oriase&gt;&lt;/s&gt;entality']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n편이시설 다양 디자인이 현대적\n\n### Response(응답):&lt;시설, 다양하다&gt; &lt;디자인, 현대적이다&gt;&lt;/s&gt;&lt;/s&gt;널, 현대적이다&gt;&lt;/s&gt;널이다&gt;&lt;/s&gt;널이다&gt;&lt;/s&gt;累板&lt;/s&gt;널, 현대적이다&gt;&lt;/s&gt;&lt;/s&gt;裏&lt;/s&gt;널이다&gt;']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n디자인\n\n### Response(응답):&lt;디자인, 좋다&gt;&lt;/s&gt; &lt;신발, 좋다&gt;&lt;/s&gt;驪道 &lt;신발, 좋다&gt;&lt;/s&gt;iventala&lt;/s&gt;ory fiseyse&lt;/s&gt;oria&lt;/s&gt;ivental&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;onyse p']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스런 이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;禮, 고급스럽다&gt;&lt;/s&gt;供養, 고급스럽다&gt;&lt;/s&gt;瑛&lt;/s&gt;瑛&lt;/s&gt;瑛&lt;/s&gt;塋, 고급스럽다&gt;&lt;/s&gt;捐帙, 고급스럽다&gt;&lt;/s&gt;nal']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n편안함\n\n### Response(응답):&lt;NULL, 편안하다&gt;&lt;/s&gt;&lt;/s&gt; &lt;이용, 편하다&gt;&lt;/s&gt; &lt;이용, 편하다&gt;&lt;/s&gt; 이단으로 규정했다.\n한다&gt;&lt;/s&gt; 이단으로 규정했다.\n, 성 신시군으로 옮겨졌다.\n 인디애나 친 계, 신시군으로 옮겼다.\n&lt;/s&gt; 신시군으로 옮겨졌다.\n&lt;/s&gt; 신시']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 느낌이 들어서\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; &lt;혜, 좋다&gt;&lt;/s&gt; &lt;신발, 좋다&gt;&lt;/s&gt;&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n이름이 좋다\n\n### Response(응답):&lt;이름, 좋다&gt;&lt;/s&gt; 후주, 후주이다&gt;&lt;/s&gt; 후주, 후주이다&gt;&lt;/s&gt; 후주이다&gt;&lt;/s&gt; 후주, 후주이다&gt;&lt;/s&gt; 초월되었다&gt;&lt;/s&gt; 초월한다&gt;&lt;/s&gt; 초월한다']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n설계가 잘되어있다\n\n### Response(응답):&lt;설계, 잘 되어 있다&gt;&lt;/s&gt;널 증상, 개선된다&gt;&lt;/s&gt;널, 개선된다&gt;&lt;/s&gt;널, 개선된다&gt;&lt;/s&gt;널, 개선된다&gt;&lt;/s&gt;裏廠裏塵, 개선된다&gt;&lt;/s&gt;西']</t>
-  </si>
-  <si>
-    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n전문가가 설계한 느낌\n\n### Response(응답):&lt;설계, 전문적이다&gt;&lt;/s&gt;敾, 전문적이다&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;樓, 전문적이다&gt;&lt;/s&gt;樓, 전문적이다&gt;&lt;/s&gt;累學界, 전문']</t>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러움\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; 꺼진다&gt;&lt;/s&gt;鏃鐵, 뚫어주는 느낌이다&gt;&lt;/s&gt; 뚫어주는 느낌이다&gt;&lt;/s&gt; 뚫어주는 느낌이다&gt;&lt;/s&gt;珠&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; &lt;仙新興, 뚫어주는 느낌이']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n디자인\n\n### Response(응답):&lt;디자인, 좋다&gt;&lt;/s&gt; 설명, 세다&gt;&lt;/s&gt; &lt;설명, 세다&gt;&lt;/s&gt;布控約束, 세다&gt;&lt;/s&gt;oria&lt;/s&gt;oria&lt;/s&gt;oria coria&lt;/s&gt;oria&lt;/s&gt;&lt;/s&gt;oria foriase delylelse']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;梨, 이롭다&gt;&lt;/s&gt; &lt;이미지, 예쁘다&gt;&lt;/s&gt;梨&lt;/s&gt;梨&lt;/s&gt;梨&lt;/s&gt;梨&lt;/s&gt;梨 향泉饗堂, 예쁘게 된다&gt;&lt;/s&gt;裏表&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n삼성이라는 브랜드\n\n### Response(응답):&lt;브랜드, 좋다&gt;&lt;/s&gt; 편하다&gt;&lt;/s&gt; 편하다&gt;&lt;/s&gt; 편하다&gt;&lt;/s&gt; 편하여&lt;/s&gt; 편하다&gt;&lt;/s&gt; 편&lt;/s&gt; 편ediay ty ty tyy ty ty fy ty c']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n전문건설업체시공\n\n### Response(응답):&lt; 업체, 전문적이다&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;&lt;/s&gt;丸, 전문적이다&gt;&lt;/s&gt;境皆&lt;/s&gt;尤&lt;/s&gt;境板&gt;&lt;/s&gt; &lt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n가장 유명한 브랜드라서\n\n### Response(응답):&lt;브랜드, 유명하다&gt;&lt;/s&gt;串, 유명하다&gt;&lt;/s&gt;串, 끗하다&gt;&lt;/s&gt;串, 끗하다&gt;&lt;/s&gt;串義&lt;/s&gt;霜&lt;/s&gt;&lt;/s&gt;牀粉&lt;/s&gt;滓泥 tople, 籤取濁池,']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n튼튼하교 깨끗\n\n### Response(응답):&lt;NULL, 튼튼하다&gt; &lt;NULL, 깨끗하다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; &lt;탁주, 친숙하다&gt;&lt;/s&gt;&lt;/s&gt; 있다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;oria']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n현대라는 회사가 믿을수 있어서\n\n### Response(응답):&lt;회사, 믿음이 간다&gt;&lt;/s&gt;裏&lt;/s&gt;裏 &lt;설계, 이조 않는다&gt;&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;履圖), 편리하다&gt;&lt;/s&gt;善&lt;/s&gt;善&lt;/s&gt;善新興通信願述撰料, 편리하다&gt;&lt;/s&gt;善)의 향圖), 편리하다']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; &lt;이용, 거부감이 없다&gt;&lt;/s&gt;oire &lt;굴, 패진다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; 후&lt;/s&gt; 후&lt;/s&gt; 후에도 인상적이다&gt;&lt;/s&gt;&lt;/s&gt;幡&lt;/s&gt; 후에&lt;/s&gt;幡&lt;/s&gt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스럽다\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;析, 들어있다&gt;&lt;/s&gt; 들어있다&gt;&lt;/s&gt;&lt;/s&gt; 들어있다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; 들어있다&gt;&lt;/s&gt;&lt;/s&gt;ut &lt;晋utoria t&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 이미지\n\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;梨 &lt;향, 고급스럽다&gt;&lt;/s&gt;ric, 고급스럽다&gt;&lt;/s&gt;entalial)&lt;/s&gt;梨&lt;/s&gt;entalica&gt;&lt;/s&gt;entalely&lt;/s&gt;entalicaely整entalica']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n편이시설 다양 디자인이 현대적\n\n### Response(응답):&lt;시설, 다양하다&gt; &lt;디자인, 현대적이다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;蛉 &lt;申竹, 과학적이다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; 있다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;ental&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n디자인\n\n### Response(응답):&lt;디자인, 좋다&gt;&lt;/s&gt;·풍척, 좋다&gt;&lt;/s&gt; &lt;향, 좋다&gt;&lt;/s&gt;&lt;/s&gt; 않는다&gt;&lt;/s&gt;境界&lt;/s&gt;境界&lt;/s&gt;境界&lt;/s&gt;&lt;/s&gt;&lt;/s&gt; Relicase Colipse&lt;/s&gt;境界&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스런 이미지\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt;泥板, 금방 깬다&gt;&lt;/s&gt;泥板, 금방 깬다&gt;&lt;/s&gt;&lt;/s&gt;泥板, 금방 깬다&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;新&lt;/s&gt;新&lt;/s&gt;新&lt;/s&gt;新']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n편안함\n\n### Response(응답):&lt;NULL, 편안하다&gt;&lt;/s&gt;梨)〉&lt;/s&gt;裏 &lt;향, 인상적이다&gt;&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt;裏&lt;/s&gt; 선혜&lt;/s&gt;&lt;/s&gt;裏&lt;/s&gt;&lt;/s&gt;裏&lt;/s&gt;裏']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n고급스러운 느낌이 들어서\n\n### Response(응답):&lt;NULL, 고급스럽다&gt;&lt;/s&gt; &lt;이미지, 좋다&gt;&lt;/s&gt; &lt;이미지, 좋다&gt;&lt;/s&gt;裏印出, 이당하고 있다&gt;&lt;/s&gt;裏決表裏表裏表裏表裏表裏表裏']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n이름이 좋다\n\n### Response(응답):&lt;이름, 좋다&gt;&lt;/s&gt;樽, 선호한다&gt;&lt;/s&gt;enz&lt;供y, 선호한다&gt;&lt;/s&gt;裏&gt;&lt;/s&gt;enzLL, 선호한다&gt;&lt;/s&gt;&lt;/s&gt;enzaLL, 선호한다&gt;&lt;/s&gt;ology&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n설계가 잘되어있다\n\n### Response(응답):&lt;설계, 잘 되어 있다&gt;&lt;/s&gt; 수취하기, 편하다&gt;&lt;/s&gt;rieel, 편하다&gt;&lt;/s&gt; 편하다&gt;&lt;/s&gt;仙&lt;/s&gt;ental fashel, 편하다&gt;&lt;/s&gt; 論&lt;/s&gt; 편하다&gt;&lt;/s&gt; Historia&lt;/s&gt; 편&lt;/s&gt;']</t>
+  </si>
+  <si>
+    <t>['Below is an instruction that describes a task, paired with an input that provides further context.\n아래는 작업을 설명하는 명령어와 추가적 맥락을 제공하는 입력이 짝을 이루는 예제입니다.\n\nWrite a response that appropriately completes the request.\n요청을 적절히 완료하는 응답을 작성하세요.\n\n### Instruction(명령어):\n다음 텍스트는 긍정적인 리뷰이다. 다음 텍스트에 대해서 &lt;속성, 의견&gt; 형태로 의견을 추출해줘.\n\n### Input(입력):\n전문가가 설계한 느낌\n\n### Response(응답):&lt;설계, 전문적이다&gt;&lt;/s&gt;臺 &lt;NULL, 신선하다&gt;&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;臺 &lt;척, 좋다&gt;&lt;/s&gt;臺)&lt;/s&gt;臺)&lt;/s&gt;']</t>
   </si>
 </sst>
 </file>

</xml_diff>